<commit_message>
Modified JSSP problems and added .gitignore
</commit_message>
<xml_diff>
--- a/JSSP-problems/abz7.xlsx
+++ b/JSSP-problems/abz7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\URV\Neural-and-Evolutionary-Computation\ACTIVITY2\A2_MarinaLopez\JSSP-problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D0CDEDB-5946-4216-A715-475CF95C638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784A1BC0-705B-47A9-9B98-EE8DE5A37F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="3420" windowWidth="38700" windowHeight="15885" xr2:uid="{7D0ACDA4-DC06-4E55-B561-A8B1465C00C7}"/>
+    <workbookView xWindow="1020" yWindow="2805" windowWidth="25770" windowHeight="17805" xr2:uid="{7D0ACDA4-DC06-4E55-B561-A8B1465C00C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,56 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
-  <si>
-    <t>2 2</t>
-  </si>
-  <si>
-    <t>3 1</t>
-  </si>
-  <si>
-    <t>9 1</t>
-  </si>
-  <si>
-    <t>4 2</t>
-  </si>
-  <si>
-    <t>0 2</t>
-  </si>
-  <si>
-    <t>6 2</t>
-  </si>
-  <si>
-    <t>8 2</t>
-  </si>
-  <si>
-    <t>7 2</t>
-  </si>
-  <si>
-    <t>1 3</t>
-  </si>
-  <si>
-    <t>5 3</t>
-  </si>
-  <si>
-    <t>1 1</t>
-  </si>
-  <si>
-    <t>8 1</t>
-  </si>
-  <si>
-    <t>4 1</t>
-  </si>
-  <si>
-    <t>6 1</t>
-  </si>
-  <si>
-    <t>3 3</t>
-  </si>
-  <si>
-    <t>0 1</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,101 +417,101 @@
   <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>24</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <v>9</v>
+      </c>
+      <c r="F1">
+        <v>17</v>
+      </c>
+      <c r="G1">
+        <v>4</v>
+      </c>
+      <c r="H1">
+        <v>27</v>
+      </c>
+      <c r="I1">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="J1">
+        <v>21</v>
+      </c>
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>25</v>
+      </c>
+      <c r="M1">
+        <v>8</v>
+      </c>
+      <c r="N1">
+        <v>27</v>
+      </c>
+      <c r="O1">
+        <v>7</v>
+      </c>
+      <c r="P1">
+        <v>26</v>
+      </c>
+      <c r="Q1">
         <v>1</v>
       </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="R1">
+        <v>30</v>
+      </c>
+      <c r="S1">
         <v>5</v>
       </c>
-      <c r="L1">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1">
-        <v>6</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1">
-        <v>0</v>
-      </c>
-      <c r="S1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="T1">
+        <v>31</v>
+      </c>
+      <c r="U1">
+        <v>11</v>
+      </c>
+      <c r="V1">
+        <v>18</v>
+      </c>
+      <c r="W1">
+        <v>14</v>
+      </c>
+      <c r="X1">
+        <v>16</v>
+      </c>
+      <c r="Y1">
+        <v>13</v>
+      </c>
+      <c r="Z1">
+        <v>39</v>
+      </c>
+      <c r="AA1">
         <v>10</v>
       </c>
-      <c r="U1" t="s">
-        <v>10</v>
-      </c>
-      <c r="V1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>0</v>
+      <c r="AB1">
+        <v>19</v>
+      </c>
+      <c r="AC1">
+        <v>12</v>
       </c>
       <c r="AD1">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:30">

</xml_diff>